<commit_message>
lots of additions and updates
</commit_message>
<xml_diff>
--- a/wind_experiment/data/old_xlsx_files/SLA_leaf_wts_2013.xlsx
+++ b/wind_experiment/data/old_xlsx_files/SLA_leaf_wts_2013.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24426"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="220" windowWidth="21360" windowHeight="15080"/>
+    <workbookView xWindow="8860" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$164</definedName>
+  </definedNames>
   <calcPr calcId="130407" concurrentCalc="0"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="169">
   <si>
     <t>plant.code</t>
   </si>
@@ -33,15 +36,6 @@
     <t>batch.no</t>
   </si>
   <si>
-    <t>1U2</t>
-  </si>
-  <si>
-    <t>1U1</t>
-  </si>
-  <si>
-    <t>3E3</t>
-  </si>
-  <si>
     <t>2u10</t>
   </si>
   <si>
@@ -264,9 +258,6 @@
     <t>8u4</t>
   </si>
   <si>
-    <t>1039</t>
-  </si>
-  <si>
     <t>4u8</t>
   </si>
   <si>
@@ -313,9 +304,6 @@
   </si>
   <si>
     <t>8u7</t>
-  </si>
-  <si>
-    <t>1036</t>
   </si>
   <si>
     <t>10u7</t>
@@ -522,15 +510,41 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9u4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>1u2</t>
+  </si>
+  <si>
+    <t>3e3</t>
+  </si>
+  <si>
+    <t>1u1</t>
+  </si>
+  <si>
+    <t>10e9</t>
+  </si>
+  <si>
+    <t>10e6</t>
+  </si>
+  <si>
+    <t>10e1</t>
+  </si>
+  <si>
+    <t>3e1</t>
+  </si>
+  <si>
+    <t>9u1</t>
+  </si>
+  <si>
+    <t>9u9</t>
+  </si>
+  <si>
+    <t>10u8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,7 +585,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -838,21 +852,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="1"/>
   </cols>
@@ -868,10 +882,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -879,7 +893,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="C2">
         <v>4.8599999999999997E-2</v>
@@ -890,7 +904,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="C3">
         <v>2.7199999999999998E-2</v>
@@ -901,7 +915,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>161</v>
       </c>
       <c r="C4">
         <v>4.48E-2</v>
@@ -912,7 +926,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>5.0700000000000002E-2</v>
@@ -923,7 +937,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>3.3599999999999998E-2</v>
@@ -934,7 +948,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>4.1099999999999998E-2</v>
@@ -945,7 +959,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>4.2200000000000001E-2</v>
@@ -956,7 +970,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>4.5600000000000002E-2</v>
@@ -967,7 +981,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>1.66E-2</v>
@@ -978,7 +992,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>2.53E-2</v>
@@ -989,7 +1003,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>5.0200000000000002E-2</v>
@@ -1000,7 +1014,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>3.0099999999999998E-2</v>
@@ -1011,7 +1025,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>4.8800000000000003E-2</v>
@@ -1022,7 +1036,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>5.8599999999999999E-2</v>
@@ -1033,7 +1047,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>2.4899999999999999E-2</v>
@@ -1044,7 +1058,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>2.81E-2</v>
@@ -1055,7 +1069,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>2.6700000000000002E-2</v>
@@ -1066,7 +1080,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>6.6600000000000006E-2</v>
@@ -1077,7 +1091,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>2.9100000000000001E-2</v>
@@ -1088,7 +1102,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>1.54E-2</v>
@@ -1099,7 +1113,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C22">
         <v>2.23E-2</v>
@@ -1110,7 +1124,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C23">
         <v>8.7400000000000005E-2</v>
@@ -1121,7 +1135,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C24">
         <v>3.7900000000000003E-2</v>
@@ -1132,7 +1146,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>15</v>
+        <v>165</v>
       </c>
       <c r="C25">
         <v>3.56E-2</v>
@@ -1143,7 +1157,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C26">
         <v>5.3900000000000003E-2</v>
@@ -1154,7 +1168,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C27">
         <v>4.4999999999999998E-2</v>
@@ -1165,7 +1179,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C28">
         <v>2.5899999999999999E-2</v>
@@ -1176,7 +1190,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C29">
         <v>5.11E-2</v>
@@ -1187,7 +1201,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C30">
         <v>1.9900000000000001E-2</v>
@@ -1198,7 +1212,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C31">
         <v>2.47E-2</v>
@@ -1209,7 +1223,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C32">
         <v>1.6799999999999999E-2</v>
@@ -1220,7 +1234,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C33">
         <v>1.43E-2</v>
@@ -1231,7 +1245,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C34">
         <v>4.5600000000000002E-2</v>
@@ -1242,7 +1256,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C35">
         <v>2.7099999999999999E-2</v>
@@ -1253,7 +1267,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C36">
         <v>2.6100000000000002E-2</v>
@@ -1264,7 +1278,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C37">
         <v>6.1699999999999998E-2</v>
@@ -1275,7 +1289,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C38">
         <v>1.9E-2</v>
@@ -1286,7 +1300,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C39">
         <v>0.44600000000000001</v>
@@ -1297,7 +1311,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C40">
         <v>1.2800000000000001E-2</v>
@@ -1308,7 +1322,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C41">
         <v>5.3499999999999999E-2</v>
@@ -1319,7 +1333,7 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C42">
         <v>4.3299999999999998E-2</v>
@@ -1330,7 +1344,7 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C43">
         <v>7.1000000000000004E-3</v>
@@ -1341,7 +1355,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C44">
         <v>2.9000000000000001E-2</v>
@@ -1352,7 +1366,7 @@
         <v>3</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C45">
         <v>3.8899999999999997E-2</v>
@@ -1363,7 +1377,7 @@
         <v>3</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C46">
         <v>6.8999999999999999E-3</v>
@@ -1374,7 +1388,7 @@
         <v>3</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C47">
         <v>6.1199999999999997E-2</v>
@@ -1385,7 +1399,7 @@
         <v>3</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C48">
         <v>2.53E-2</v>
@@ -1396,7 +1410,7 @@
         <v>3</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C49">
         <v>6.1800000000000001E-2</v>
@@ -1407,7 +1421,7 @@
         <v>3</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C50">
         <v>0.03</v>
@@ -1418,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C51">
         <v>1.1299999999999999E-2</v>
@@ -1429,7 +1443,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C52">
         <v>2.18E-2</v>
@@ -1440,7 +1454,7 @@
         <v>3</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C53">
         <v>4.2700000000000002E-2</v>
@@ -1451,7 +1465,7 @@
         <v>3</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C54">
         <v>2.8500000000000001E-2</v>
@@ -1462,7 +1476,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C55">
         <v>9.7000000000000003E-3</v>
@@ -1473,7 +1487,7 @@
         <v>3</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C56">
         <v>2.1499999999999998E-2</v>
@@ -1484,7 +1498,7 @@
         <v>3</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C57">
         <v>7.8E-2</v>
@@ -1495,7 +1509,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C58">
         <v>2.2800000000000001E-2</v>
@@ -1506,7 +1520,7 @@
         <v>3</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C59">
         <v>2.7799999999999998E-2</v>
@@ -1517,7 +1531,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C60">
         <v>3.4200000000000001E-2</v>
@@ -1528,7 +1542,7 @@
         <v>3</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C61">
         <v>1.89E-2</v>
@@ -1539,7 +1553,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C62">
         <v>4.7E-2</v>
@@ -1550,7 +1564,7 @@
         <v>3</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C63">
         <v>6.9900000000000004E-2</v>
@@ -1561,7 +1575,7 @@
         <v>3</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C64">
         <v>1.7899999999999999E-2</v>
@@ -1572,7 +1586,7 @@
         <v>3</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C65">
         <v>2.6800000000000001E-2</v>
@@ -1583,7 +1597,7 @@
         <v>3</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C66">
         <v>1.0200000000000001E-2</v>
@@ -1594,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C67">
         <v>1.0800000000000001E-2</v>
@@ -1605,7 +1619,7 @@
         <v>3</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C68">
         <v>1.8499999999999999E-2</v>
@@ -1616,7 +1630,7 @@
         <v>3</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C69">
         <v>1.1299999999999999E-2</v>
@@ -1627,7 +1641,7 @@
         <v>3</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C70">
         <v>1.2800000000000001E-2</v>
@@ -1638,7 +1652,7 @@
         <v>3</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C71">
         <v>8.6999999999999994E-3</v>
@@ -1649,7 +1663,7 @@
         <v>3</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C72">
         <v>1.09E-2</v>
@@ -1660,7 +1674,7 @@
         <v>3</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C73">
         <v>1.11E-2</v>
@@ -1671,7 +1685,7 @@
         <v>3</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C74">
         <v>3.5900000000000001E-2</v>
@@ -1682,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C75">
         <v>4.3700000000000003E-2</v>
@@ -1693,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C76">
         <v>2.9000000000000001E-2</v>
@@ -1704,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C77">
         <v>2.4400000000000002E-2</v>
@@ -1715,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C78">
         <v>4.7699999999999999E-2</v>
@@ -1726,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C79">
         <v>3.5999999999999997E-2</v>
@@ -1737,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C80">
         <v>2.86E-2</v>
@@ -1748,7 +1762,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>80</v>
+        <v>162</v>
       </c>
       <c r="C81">
         <v>1.6299999999999999E-2</v>
@@ -1759,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C82">
         <v>1.84E-2</v>
@@ -1770,7 +1784,7 @@
         <v>1</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C83">
         <v>3.9E-2</v>
@@ -1781,7 +1795,7 @@
         <v>1</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C84">
         <v>4.1599999999999998E-2</v>
@@ -1792,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C85">
         <v>2.23E-2</v>
@@ -1803,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>77</v>
+        <v>166</v>
       </c>
       <c r="C86">
         <v>1.9800000000000002E-2</v>
@@ -1814,7 +1828,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C87">
         <v>1.47E-2</v>
@@ -1825,7 +1839,7 @@
         <v>1</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C88">
         <v>3.7400000000000003E-2</v>
@@ -1836,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C89">
         <v>2.9600000000000001E-2</v>
@@ -1847,7 +1861,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C90">
         <v>3.9699999999999999E-2</v>
@@ -1858,7 +1872,7 @@
         <v>1</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C91">
         <v>1.55E-2</v>
@@ -1869,7 +1883,7 @@
         <v>1</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C92">
         <v>1.3100000000000001E-2</v>
@@ -1880,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C93">
         <v>1.8100000000000002E-2</v>
@@ -1891,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C94">
         <v>1.46E-2</v>
@@ -1902,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C95">
         <v>3.4799999999999998E-2</v>
@@ -1913,7 +1927,7 @@
         <v>1</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C96">
         <v>2.8299999999999999E-2</v>
@@ -1924,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C97">
         <v>1.4999999999999999E-2</v>
@@ -1935,7 +1949,7 @@
         <v>1</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C98">
         <v>1.2200000000000001E-2</v>
@@ -1946,7 +1960,7 @@
         <v>1</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>97</v>
+        <v>163</v>
       </c>
       <c r="C99">
         <v>6.7000000000000002E-3</v>
@@ -1957,7 +1971,7 @@
         <v>1</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C100">
         <v>3.2000000000000002E-3</v>
@@ -1968,7 +1982,7 @@
         <v>1</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C101">
         <v>8.8999999999999999E-3</v>
@@ -1979,7 +1993,7 @@
         <v>1</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C102">
         <v>6.7999999999999996E-3</v>
@@ -1990,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C103">
         <v>4.3299999999999998E-2</v>
@@ -2001,7 +2015,7 @@
         <v>1</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C104">
         <v>3.0000000000000001E-3</v>
@@ -2012,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C105">
         <v>5.7000000000000002E-3</v>
@@ -2023,7 +2037,7 @@
         <v>1</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C106">
         <v>6.4000000000000003E-3</v>
@@ -2032,7 +2046,7 @@
         <v>1</v>
       </c>
       <c r="E106" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2040,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C107">
         <v>7.6E-3</v>
@@ -2049,7 +2063,7 @@
         <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2057,7 +2071,7 @@
         <v>2</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C108">
         <v>1.47E-2</v>
@@ -2068,7 +2082,7 @@
         <v>2</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C109">
         <v>3.6600000000000001E-2</v>
@@ -2079,7 +2093,7 @@
         <v>2</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C110">
         <v>1.3899999999999999E-2</v>
@@ -2090,7 +2104,7 @@
         <v>2</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C111">
         <v>3.09E-2</v>
@@ -2101,7 +2115,7 @@
         <v>2</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C112">
         <v>2.41E-2</v>
@@ -2112,7 +2126,7 @@
         <v>2</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C113">
         <v>2.5899999999999999E-2</v>
@@ -2123,7 +2137,7 @@
         <v>2</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C114">
         <v>2.9600000000000001E-2</v>
@@ -2134,7 +2148,7 @@
         <v>2</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C115">
         <v>2.4500000000000001E-2</v>
@@ -2145,7 +2159,7 @@
         <v>2</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C116">
         <v>3.5999999999999997E-2</v>
@@ -2156,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C117">
         <v>5.2400000000000002E-2</v>
@@ -2167,7 +2181,7 @@
         <v>2</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C118">
         <v>3.4200000000000001E-2</v>
@@ -2178,7 +2192,7 @@
         <v>2</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C119">
         <v>4.24E-2</v>
@@ -2189,7 +2203,7 @@
         <v>2</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C120">
         <v>2.5700000000000001E-2</v>
@@ -2200,7 +2214,7 @@
         <v>2</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C121">
         <v>2.3E-2</v>
@@ -2211,7 +2225,7 @@
         <v>2</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C122">
         <v>1.7500000000000002E-2</v>
@@ -2222,7 +2236,7 @@
         <v>2</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C123">
         <v>0.01</v>
@@ -2233,7 +2247,7 @@
         <v>2</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C124">
         <v>2.63E-2</v>
@@ -2244,7 +2258,7 @@
         <v>2</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C125">
         <v>2.1700000000000001E-2</v>
@@ -2255,7 +2269,7 @@
         <v>2</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C126">
         <v>2.5399999999999999E-2</v>
@@ -2266,7 +2280,7 @@
         <v>2</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C127">
         <v>1.8200000000000001E-2</v>
@@ -2277,7 +2291,7 @@
         <v>2</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C128">
         <v>3.3099999999999997E-2</v>
@@ -2288,7 +2302,7 @@
         <v>2</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C129">
         <v>8.2000000000000007E-3</v>
@@ -2299,7 +2313,7 @@
         <v>2</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C130">
         <v>2.5399999999999999E-2</v>
@@ -2310,7 +2324,7 @@
         <v>2</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C131">
         <v>2.3599999999999999E-2</v>
@@ -2321,7 +2335,7 @@
         <v>2</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>74</v>
+        <v>164</v>
       </c>
       <c r="C132">
         <v>1.01E-2</v>
@@ -2332,7 +2346,7 @@
         <v>2</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C133">
         <v>1.7899999999999999E-2</v>
@@ -2343,7 +2357,7 @@
         <v>2</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C134">
         <v>4.0000000000000001E-3</v>
@@ -2352,7 +2366,7 @@
         <v>1</v>
       </c>
       <c r="E134" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -2360,7 +2374,7 @@
         <v>2</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C135">
         <v>1.78E-2</v>
@@ -2371,16 +2385,13 @@
         <v>2</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C136">
         <v>1.4E-2</v>
       </c>
-      <c r="D136">
-        <v>1</v>
-      </c>
       <c r="E136" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -2388,7 +2399,7 @@
         <v>2</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C137">
         <v>2.1299999999999999E-2</v>
@@ -2399,7 +2410,7 @@
         <v>2</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C138">
         <v>2.1499999999999998E-2</v>
@@ -2407,7 +2418,7 @@
     </row>
     <row r="139" spans="1:5">
       <c r="B139" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C139">
         <v>1.2500000000000001E-2</v>
@@ -2415,7 +2426,7 @@
     </row>
     <row r="140" spans="1:5">
       <c r="B140" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C140">
         <v>6.4000000000000003E-3</v>
@@ -2423,7 +2434,7 @@
     </row>
     <row r="141" spans="1:5">
       <c r="B141" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C141">
         <v>4.5999999999999999E-3</v>
@@ -2431,7 +2442,7 @@
     </row>
     <row r="142" spans="1:5">
       <c r="B142" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C142">
         <v>3.0000000000000001E-3</v>
@@ -2439,7 +2450,7 @@
     </row>
     <row r="143" spans="1:5">
       <c r="B143" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C143">
         <v>8.6E-3</v>
@@ -2447,7 +2458,7 @@
     </row>
     <row r="144" spans="1:5">
       <c r="B144" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C144">
         <v>1.0999999999999999E-2</v>
@@ -2455,7 +2466,7 @@
     </row>
     <row r="145" spans="1:3">
       <c r="B145" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C145">
         <v>4.3E-3</v>
@@ -2463,7 +2474,7 @@
     </row>
     <row r="146" spans="1:3">
       <c r="B146" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C146">
         <v>4.4999999999999997E-3</v>
@@ -2471,7 +2482,7 @@
     </row>
     <row r="147" spans="1:3">
       <c r="B147" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C147">
         <v>1.01E-2</v>
@@ -2479,7 +2490,7 @@
     </row>
     <row r="148" spans="1:3">
       <c r="B148" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C148">
         <v>1.1999999999999999E-3</v>
@@ -2487,7 +2498,7 @@
     </row>
     <row r="149" spans="1:3">
       <c r="B149" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C149">
         <v>3.0000000000000001E-3</v>
@@ -2495,7 +2506,7 @@
     </row>
     <row r="150" spans="1:3">
       <c r="B150" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C150">
         <v>5.3E-3</v>
@@ -2503,7 +2514,7 @@
     </row>
     <row r="151" spans="1:3">
       <c r="B151" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C151">
         <v>4.1000000000000003E-3</v>
@@ -2511,7 +2522,7 @@
     </row>
     <row r="152" spans="1:3">
       <c r="B152" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C152">
         <v>4.4000000000000003E-3</v>
@@ -2519,7 +2530,7 @@
     </row>
     <row r="153" spans="1:3">
       <c r="B153" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C153">
         <v>4.0000000000000001E-3</v>
@@ -2530,7 +2541,7 @@
         <v>5</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C154">
         <v>8.3999999999999995E-3</v>
@@ -2541,7 +2552,7 @@
         <v>5</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C155">
         <v>9.9000000000000008E-3</v>
@@ -2552,7 +2563,7 @@
         <v>5</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C156">
         <v>2.3300000000000001E-2</v>
@@ -2563,7 +2574,7 @@
         <v>5</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C157">
         <v>8.6E-3</v>
@@ -2574,7 +2585,7 @@
         <v>5</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C158">
         <v>1.4800000000000001E-2</v>
@@ -2585,7 +2596,7 @@
         <v>5</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C159">
         <v>1.9400000000000001E-2</v>
@@ -2596,7 +2607,7 @@
         <v>5</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C160">
         <v>1.43E-2</v>
@@ -2607,7 +2618,7 @@
         <v>5</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C161">
         <v>8.9999999999999993E-3</v>
@@ -2618,7 +2629,7 @@
         <v>5</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C162">
         <v>7.9000000000000008E-3</v>
@@ -2629,7 +2640,7 @@
         <v>5</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C163">
         <v>1.46E-2</v>
@@ -2640,18 +2651,19 @@
         <v>5</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C164">
         <v>1.29E-2</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E164"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>